<commit_message>
Update figures manuscript with absolute n
</commit_message>
<xml_diff>
--- a/StudyListDataBaseReExtraction.xlsx
+++ b/StudyListDataBaseReExtraction.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\Videos\From_github\SRPolicy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A23B9FF-4D2D-4CBB-8FB0-51D9BEF3ADD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04C6074-711E-4EE3-8134-C39BFB322E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="102">
   <si>
     <t>StudyId</t>
   </si>
@@ -320,6 +320,12 @@
   </si>
   <si>
     <t>Assessment of the control measures of the category A diseases of Animal Health Law: Rift Valley Fever</t>
+  </si>
+  <si>
+    <t>no?</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
@@ -702,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1072,6 +1078,9 @@
       <c r="C25" t="s">
         <v>4</v>
       </c>
+      <c r="D25" t="s">
+        <v>4</v>
+      </c>
       <c r="E25" t="s">
         <v>51</v>
       </c>
@@ -1144,6 +1153,9 @@
       <c r="C30" t="s">
         <v>4</v>
       </c>
+      <c r="D30" t="s">
+        <v>4</v>
+      </c>
       <c r="E30" t="s">
         <v>61</v>
       </c>
@@ -1156,6 +1168,9 @@
       <c r="C31" t="s">
         <v>4</v>
       </c>
+      <c r="D31" t="s">
+        <v>100</v>
+      </c>
       <c r="E31" t="s">
         <v>63</v>
       </c>
@@ -1168,6 +1183,9 @@
       <c r="C32" t="s">
         <v>4</v>
       </c>
+      <c r="D32" t="s">
+        <v>4</v>
+      </c>
       <c r="E32" t="s">
         <v>65</v>
       </c>
@@ -1180,6 +1198,9 @@
       <c r="C33" t="s">
         <v>4</v>
       </c>
+      <c r="D33" t="s">
+        <v>4</v>
+      </c>
       <c r="E33" t="s">
         <v>67</v>
       </c>
@@ -1192,6 +1213,9 @@
       <c r="C34" t="s">
         <v>4</v>
       </c>
+      <c r="D34" t="s">
+        <v>4</v>
+      </c>
       <c r="E34" t="s">
         <v>69</v>
       </c>
@@ -1204,6 +1228,9 @@
       <c r="C35" t="s">
         <v>4</v>
       </c>
+      <c r="D35" t="s">
+        <v>4</v>
+      </c>
       <c r="E35" t="s">
         <v>71</v>
       </c>
@@ -1216,6 +1243,9 @@
       <c r="C36" t="s">
         <v>4</v>
       </c>
+      <c r="D36" t="s">
+        <v>101</v>
+      </c>
       <c r="E36" t="s">
         <v>73</v>
       </c>
@@ -1228,6 +1258,9 @@
       <c r="C37" t="s">
         <v>4</v>
       </c>
+      <c r="D37" t="s">
+        <v>4</v>
+      </c>
       <c r="E37" t="s">
         <v>75</v>
       </c>
@@ -1240,6 +1273,9 @@
       <c r="C38" t="s">
         <v>4</v>
       </c>
+      <c r="D38" t="s">
+        <v>4</v>
+      </c>
       <c r="E38" t="s">
         <v>77</v>
       </c>
@@ -1252,6 +1288,9 @@
       <c r="C39" t="s">
         <v>4</v>
       </c>
+      <c r="D39" t="s">
+        <v>4</v>
+      </c>
       <c r="E39" t="s">
         <v>79</v>
       </c>
@@ -1264,6 +1303,9 @@
       <c r="C40" t="s">
         <v>4</v>
       </c>
+      <c r="D40" t="s">
+        <v>4</v>
+      </c>
       <c r="E40" t="s">
         <v>81</v>
       </c>
@@ -1276,6 +1318,9 @@
       <c r="C41" t="s">
         <v>4</v>
       </c>
+      <c r="D41" t="s">
+        <v>4</v>
+      </c>
       <c r="E41" t="s">
         <v>83</v>
       </c>
@@ -1288,6 +1333,9 @@
       <c r="C42" t="s">
         <v>4</v>
       </c>
+      <c r="D42" t="s">
+        <v>4</v>
+      </c>
       <c r="E42" t="s">
         <v>85</v>
       </c>
@@ -1300,6 +1348,9 @@
       <c r="C43" t="s">
         <v>4</v>
       </c>
+      <c r="D43" t="s">
+        <v>4</v>
+      </c>
       <c r="E43" t="s">
         <v>87</v>
       </c>
@@ -1312,6 +1363,9 @@
       <c r="C44" t="s">
         <v>4</v>
       </c>
+      <c r="D44" t="s">
+        <v>4</v>
+      </c>
       <c r="E44" t="s">
         <v>89</v>
       </c>
@@ -1324,6 +1378,9 @@
       <c r="C45" t="s">
         <v>4</v>
       </c>
+      <c r="D45" t="s">
+        <v>4</v>
+      </c>
       <c r="E45" t="s">
         <v>91</v>
       </c>
@@ -1336,6 +1393,9 @@
       <c r="C46" t="s">
         <v>4</v>
       </c>
+      <c r="D46" t="s">
+        <v>4</v>
+      </c>
       <c r="E46" t="s">
         <v>93</v>
       </c>
@@ -1348,6 +1408,9 @@
       <c r="C47" t="s">
         <v>4</v>
       </c>
+      <c r="D47" t="s">
+        <v>4</v>
+      </c>
       <c r="E47" t="s">
         <v>95</v>
       </c>
@@ -1360,6 +1423,9 @@
       <c r="C48" t="s">
         <v>4</v>
       </c>
+      <c r="D48" t="s">
+        <v>4</v>
+      </c>
       <c r="E48" t="s">
         <v>97</v>
       </c>
@@ -1372,6 +1438,9 @@
       <c r="C49" t="s">
         <v>4</v>
       </c>
+      <c r="D49" t="s">
+        <v>4</v>
+      </c>
       <c r="E49" t="s">
         <v>99</v>
       </c>

</xml_diff>